<commit_message>
Updated external XML schema and files.
</commit_message>
<xml_diff>
--- a/static_files/Externals.xlsx
+++ b/static_files/Externals.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="19035" windowHeight="10995"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="15480" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Description</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>ID (calculated)</t>
-  </si>
-  <si>
-    <t>DisplayName (calculated)</t>
   </si>
   <si>
     <t>Victorian Institute of Sport (VIS)</t>
@@ -67,15 +64,67 @@
     <t>Organisation</t>
   </si>
   <si>
-    <t>Name of School/Department/Group
-(ideally leave blank)</t>
+    <t>University of Ballarat</t>
+  </si>
+  <si>
+    <t>The University of Ballarat (UB) is Australia's only regional, multi-sector university. We are the third oldest site of higher learning in Australia, and offer secondary schooling, TAFE, higher education, and research opportunities. We have campuses in Ballarat, Horsham, Stawell and Ararat. We also work with a range of partner institutes across Australia and the world.
+UB has around 23,000 international and domestic students. We are committed to serving regional Victorian communities, yet have a broad national and international outlook. UB offers the best of both worlds; combining a strong tradition of 142 years of tertiary education with the freedom and dynamism that comes with being a multi-sector University with close links to local industry and technology.</t>
+  </si>
+  <si>
+    <t>http://www.ballarat.edu.au/</t>
+  </si>
+  <si>
+    <t>P.O. Box 663. Ballarat VIC 3353</t>
+  </si>
+  <si>
+    <t>+61 3 5327 9000</t>
+  </si>
+  <si>
+    <t>Swiss Federal Institute of Technology (Zurich ETH)</t>
+  </si>
+  <si>
+    <t>Consistently ranked the top university in continental Europe, ETH Zurich, the Swiss Federal Institute of Technology, is a leading player in research and education in Switzerland and worldwide. ETH Zurich's 16 departments offer Bachelor, Master and Doctoral programmes in engineering and natural sciences. The language of instruction in the Bachelor programmes is German, whereas English is the lingua franca on the graduate level. All degree programmes provide a solid scientific foundation combined with outstanding all-round skills, equipping ETH graduates with the abilities and flexibility needed for a career in industry, business or the public sector, as entrepreneur or scientist.</t>
+  </si>
+  <si>
+    <t>Weinbergstrasse 56/58
+8092 Zurich
+Switzerland</t>
+  </si>
+  <si>
+    <t>+41 43 499 60 80</t>
+  </si>
+  <si>
+    <t>http://www.ethz.ch/index_EN</t>
+  </si>
+  <si>
+    <t>GWMWater</t>
+  </si>
+  <si>
+    <t>Grampians / Wimmera / Mallee Water is a government owned water business responsible for managing water and waste supply systems in the Grampians, Wimmera and Mallee regions of Western Victoria.</t>
+  </si>
+  <si>
+    <t>http://www.gwmwater.org.au/</t>
+  </si>
+  <si>
+    <t>PO Box 481
+Horsham Vic 3402</t>
+  </si>
+  <si>
+    <t>1300 659 961
++61 3 5382 4611</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>DisplayName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +162,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -138,7 +193,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -166,9 +221,36 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -283,6 +365,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -301,7 +384,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -391,7 +474,7 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema1">
+  <Schema ID="Schema2">
     <xs:schema xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns="" elementFormDefault="qualified">
       <xs:element name="Departments">
         <xs:complexType>
@@ -399,9 +482,8 @@
             <xs:element name="Department">
               <xs:complexType>
                 <xs:sequence>
-                  <xs:element name="Name" type="xs:string"/>
+                  <xs:element name="Key" type="xs:string"/>
                   <xs:element name="DisplayName" type="xs:string"/>
-                  <xs:element name="Faculty" type="xs:string"/>
                   <xs:element name="Description" type="xs:string"/>
                   <xs:element name="Website" type="xs:anyURI"/>
                   <xs:element name="Email" type="xs:string">
@@ -417,13 +499,13 @@
       </xs:element>
     </xs:schema>
   </Schema>
-  <Map ID="5" Name="Departments_Map" RootElement="Departments" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="6" Name="Departments_Map" RootElement="Departments" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="38" name="Table38" displayName="Table38" ref="A1:I2" tableType="xml" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="38" name="Table38" displayName="Table38" ref="A1:I5" tableType="xml" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I5">
     <filterColumn colId="0"/>
     <filterColumn colId="1"/>
     <filterColumn colId="3"/>
@@ -434,34 +516,34 @@
     <filterColumn colId="8"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="3" uniqueName="Faculty" name="Organisation" dataDxfId="8">
-      <xmlColumnPr mapId="5" xpath="/Departments/Department/Faculty" xmlDataType="string"/>
+    <tableColumn id="3" uniqueName="id" name="Organisation" dataDxfId="8">
+      <xmlColumnPr mapId="6" xpath="/Departments/Department/@id" xmlDataType="anyType"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Name" name="Name of School/Department/Group_x000a_(ideally leave blank)" dataDxfId="7">
-      <xmlColumnPr mapId="5" xpath="/Departments/Department/Name" xmlDataType="string"/>
+    <tableColumn id="2" uniqueName="Key" name="Key" dataDxfId="7">
+      <calculatedColumnFormula>1000+ROW(B2)</calculatedColumnFormula>
+      <xmlColumnPr mapId="6" xpath="/Departments/Department/Key" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="1" uniqueName="id" name="ID (calculated)" dataDxfId="6" dataCellStyle="Normal">
-      <calculatedColumnFormula>UPPER(IF(B2="",A2,(B2&amp;" - "&amp;A2)))</calculatedColumnFormula>
-      <xmlColumnPr mapId="5" xpath="/Departments/Department/@id" xmlDataType="anyType"/>
+      <calculatedColumnFormula>UPPER(A2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" uniqueName="DisplayName" name="DisplayName (calculated)" dataDxfId="5" dataCellStyle="Normal">
+    <tableColumn id="9" uniqueName="DisplayName" name="DisplayName" dataDxfId="5" dataCellStyle="Normal">
       <calculatedColumnFormula>PROPER(IF(B2="",A2,(B2&amp;", "&amp;A2)))</calculatedColumnFormula>
-      <xmlColumnPr mapId="5" xpath="/Departments/Department/DisplayName" xmlDataType="string"/>
+      <xmlColumnPr mapId="6" xpath="/Departments/Department/DisplayName" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="Description" name="Description" dataDxfId="4" dataCellStyle="Normal">
-      <xmlColumnPr mapId="5" xpath="/Departments/Department/Description" xmlDataType="string"/>
+      <xmlColumnPr mapId="6" xpath="/Departments/Department/Description" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="Website" name="Website" dataDxfId="3">
-      <xmlColumnPr mapId="5" xpath="/Departments/Department/Website" xmlDataType="anyURI"/>
+      <xmlColumnPr mapId="6" xpath="/Departments/Department/Website" xmlDataType="anyURI"/>
     </tableColumn>
     <tableColumn id="6" uniqueName="Email" name="Email" dataDxfId="2">
-      <xmlColumnPr mapId="5" xpath="/Departments/Department/Email" xmlDataType="string"/>
+      <xmlColumnPr mapId="6" xpath="/Departments/Department/Email" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="7" uniqueName="Address" name="Address" dataDxfId="1">
-      <xmlColumnPr mapId="5" xpath="/Departments/Department/Address" xmlDataType="string"/>
+      <xmlColumnPr mapId="6" xpath="/Departments/Department/Address" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="8" uniqueName="Phone" name="Phone" dataDxfId="0">
-      <xmlColumnPr mapId="5" xpath="/Departments/Department/Phone" xmlDataType="string"/>
+      <xmlColumnPr mapId="6" xpath="/Departments/Department/Phone" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -753,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.7109375" defaultRowHeight="15"/>
@@ -766,24 +848,24 @@
     <col min="3" max="4" width="43.7109375" style="7" customWidth="1"/>
     <col min="5" max="5" width="55.85546875" style="9" customWidth="1"/>
     <col min="6" max="6" width="26.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="5" customWidth="1"/>
     <col min="8" max="8" width="37.42578125" style="5" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" style="3" customWidth="1"/>
     <col min="10" max="16384" width="33.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="31.5">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="15.75">
       <c r="A1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>0</v>
@@ -810,45 +892,135 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="225">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="60">
+      <c r="A2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="20">
+        <f>1000+ROW(B2)</f>
+        <v>1002</v>
+      </c>
+      <c r="C2" s="20" t="str">
+        <f t="shared" ref="C2:C5" si="0">UPPER(A2)</f>
+        <v>GWMWATER</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="45">
+      <c r="A3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="20">
+        <f t="shared" ref="B3:B5" si="1">1000+ROW(B3)</f>
+        <v>1003</v>
+      </c>
+      <c r="C3" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>SWISS FEDERAL INSTITUTE OF TECHNOLOGY (ZURICH ETH)</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1">
+      <c r="A4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="20">
+        <f t="shared" si="1"/>
+        <v>1004</v>
+      </c>
+      <c r="C4" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>UNIVERSITY OF BALLARAT</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="20">
+        <f t="shared" si="1"/>
+        <v>1005</v>
+      </c>
+      <c r="C5" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>VICTORIAN INSTITUTE OF SPORT (VIS)</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="7" t="str">
-        <f t="shared" ref="C2" si="0">UPPER(IF(B2="",A2,(B2&amp;" - "&amp;A2)))</f>
-        <v>VICTORIAN INSTITUTE OF SPORT (VIS)</v>
-      </c>
-      <c r="D2" s="7" t="str">
-        <f>PROPER(IF(B2="",A2,(B2&amp;", "&amp;A2)))</f>
-        <v>Victorian Institute Of Sport (Vis)</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="F5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="I5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+    <row r="6" spans="1:12">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F5" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>